<commit_message>
-- Updated improving FPS
</commit_message>
<xml_diff>
--- a/reports/report_2025-11-30.xlsx
+++ b/reports/report_2025-11-30.xlsx
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -537,11 +537,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>1</v>
@@ -591,10 +591,10 @@
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -604,10 +604,10 @@
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -919,13 +919,13 @@
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1146,7 +1146,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26-45</t>
+          <t>13-25</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
-- Updated Real-Time streamlit web interface.
</commit_message>
<xml_diff>
--- a/reports/report_2025-11-30.xlsx
+++ b/reports/report_2025-11-30.xlsx
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -541,10 +541,10 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>2</v>
@@ -919,13 +919,13 @@
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -935,10 +935,10 @@
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>0</v>
@@ -951,13 +951,13 @@
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="19">
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-- Updated Report male and female correctly
</commit_message>
<xml_diff>
--- a/reports/report_2025-11-30.xlsx
+++ b/reports/report_2025-11-30.xlsx
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -537,14 +537,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -591,10 +591,10 @@
         </is>
       </c>
       <c r="B16" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -951,13 +951,13 @@
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="19">
@@ -1083,7 +1083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1124,32 +1124,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Age Distribution (IN)</t>
-        </is>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
+          <t>Age Distribution (IN)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
           <t>Age Group</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>13-25</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t>26-45</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>